<commit_message>
moving file html to app
</commit_message>
<xml_diff>
--- a/daftar kelompok.xlsx
+++ b/daftar kelompok.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FASTIKOM\KULIAH\PEMROGRAMAN FRAMEWORK\2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WWW\aplikasi-keuangan-kampus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="smt 6-1" sheetId="2" r:id="rId1"/>
@@ -2175,11 +2175,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2990,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>